<commit_message>
almost done with report. last minute proofreading
</commit_message>
<xml_diff>
--- a/FinalReportDraft/Kelp Samples.xlsx
+++ b/FinalReportDraft/Kelp Samples.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="149">
   <si>
     <t>Sample Number</t>
   </si>
@@ -521,14 +521,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1414,11 +1413,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2126705288"/>
-        <c:axId val="2124616376"/>
+        <c:axId val="-2130670920"/>
+        <c:axId val="-2130676312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126705288"/>
+        <c:axId val="-2130670920"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1452,7 +1451,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124616376"/>
+        <c:crossAx val="-2130676312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1460,7 +1459,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124616376"/>
+        <c:axId val="-2130676312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1512,7 +1511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126705288"/>
+        <c:crossAx val="-2130670920"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2432,11 +2431,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2125843304"/>
-        <c:axId val="2125849288"/>
+        <c:axId val="-2128178232"/>
+        <c:axId val="-2128172392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125843304"/>
+        <c:axId val="-2128178232"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2470,7 +2469,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125849288"/>
+        <c:crossAx val="-2128172392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2478,7 +2477,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125849288"/>
+        <c:axId val="-2128172392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2529,7 +2528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125843304"/>
+        <c:crossAx val="-2128178232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3443,11 +3442,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2126613512"/>
-        <c:axId val="2126612040"/>
+        <c:axId val="-2127995288"/>
+        <c:axId val="-2127989304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126613512"/>
+        <c:axId val="-2127995288"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3481,7 +3480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126612040"/>
+        <c:crossAx val="-2127989304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3489,7 +3488,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126612040"/>
+        <c:axId val="-2127989304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3541,7 +3540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126613512"/>
+        <c:crossAx val="-2127995288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3989,11 +3988,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J19" sqref="J19"/>
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4004,7 +4003,7 @@
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4035,11 +4034,8 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4070,11 +4066,8 @@
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1">
-        <v>3.7600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4106,7 +4099,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4137,11 +4130,8 @@
       <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="1">
-        <v>6.3E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4173,7 +4163,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4205,7 +4195,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4237,7 +4227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4268,11 +4258,8 @@
       <c r="J8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="1">
-        <v>7.5399999999999995E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4303,11 +4290,8 @@
       <c r="J9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="1">
-        <v>0.1137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4339,7 +4323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -4370,11 +4354,8 @@
       <c r="J11" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K11" s="4">
-        <v>6.0600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4405,11 +4386,8 @@
       <c r="J12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K12" s="1">
-        <v>7.3999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -4440,9 +4418,8 @@
       <c r="J13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -4473,11 +4450,8 @@
       <c r="J14" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K14" s="4">
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -4508,9 +4482,8 @@
       <c r="J15" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1">
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -4540,9 +4513,6 @@
       </c>
       <c r="J16" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="K16" s="4">
-        <v>3.0499999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4845,247 +4815,247 @@
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
     </row>
     <row r="22" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B30" s="7"/>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B34" s="7"/>
+      <c r="B34" s="6"/>
     </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B35" s="7"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B36" s="7"/>
+      <c r="B36" s="6"/>
     </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B37" s="7"/>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B39" s="7"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B40" s="7"/>
+      <c r="B40" s="6"/>
     </row>
     <row r="41" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B41" s="7"/>
+      <c r="B41" s="6"/>
     </row>
     <row r="42" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B42" s="7"/>
+      <c r="B42" s="6"/>
     </row>
     <row r="43" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B43" s="7"/>
+      <c r="B43" s="6"/>
     </row>
     <row r="44" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B44" s="7"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B45" s="7"/>
+      <c r="B45" s="6"/>
     </row>
     <row r="46" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B46" s="7"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B48" s="7"/>
+      <c r="B48" s="6"/>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B49" s="7"/>
+      <c r="B49" s="6"/>
     </row>
     <row r="50" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B50" s="7"/>
+      <c r="B50" s="6"/>
     </row>
     <row r="51" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
     </row>
     <row r="52" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B52" s="7"/>
+      <c r="B52" s="6"/>
     </row>
     <row r="53" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B53" s="7"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B54" s="7"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B55" s="7"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B56" s="7"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B57" s="7"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B58" s="7"/>
+      <c r="B58" s="6"/>
     </row>
     <row r="59" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B59" s="7"/>
+      <c r="B59" s="6"/>
     </row>
     <row r="60" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B60" s="7"/>
+      <c r="B60" s="6"/>
     </row>
     <row r="61" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B61" s="7"/>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B62" s="7"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B63" s="7"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B64" s="7"/>
+      <c r="B64" s="6"/>
     </row>
     <row r="65" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B65" s="7"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B66" s="7"/>
+      <c r="B66" s="6"/>
     </row>
     <row r="67" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B67" s="7"/>
+      <c r="B67" s="6"/>
     </row>
     <row r="68" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B68" s="7"/>
+      <c r="B68" s="6"/>
     </row>
     <row r="69" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B69" s="7"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B70" s="7"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B71" s="7"/>
+      <c r="B71" s="6"/>
     </row>
     <row r="72" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B72" s="7"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B73" s="7"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B74" s="7"/>
+      <c r="B74" s="6"/>
     </row>
     <row r="75" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B75" s="7"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B76" s="7"/>
+      <c r="B76" s="6"/>
     </row>
     <row r="77" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B77" s="7"/>
+      <c r="B77" s="6"/>
     </row>
     <row r="78" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B78" s="7"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B79" s="7"/>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B80" s="7"/>
+      <c r="B80" s="6"/>
     </row>
     <row r="81" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B81" s="7"/>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B82" s="7"/>
+      <c r="B82" s="6"/>
     </row>
     <row r="83" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B83" s="7"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B84" s="7"/>
+      <c r="B84" s="6"/>
     </row>
     <row r="85" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B85" s="7"/>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B86" s="7"/>
+      <c r="B86" s="6"/>
     </row>
     <row r="87" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B87" s="7"/>
+      <c r="B87" s="6"/>
     </row>
     <row r="88" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B88" s="7"/>
+      <c r="B88" s="6"/>
     </row>
     <row r="89" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B89" s="7"/>
+      <c r="B89" s="6"/>
     </row>
     <row r="90" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B90" s="7"/>
+      <c r="B90" s="6"/>
     </row>
     <row r="91" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B91" s="7"/>
+      <c r="B91" s="6"/>
     </row>
     <row r="92" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B92" s="7"/>
+      <c r="B92" s="6"/>
     </row>
     <row r="93" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B93" s="7"/>
+      <c r="B93" s="6"/>
     </row>
     <row r="94" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B94" s="7"/>
+      <c r="B94" s="6"/>
     </row>
     <row r="95" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B95" s="7"/>
+      <c r="B95" s="6"/>
     </row>
     <row r="96" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B96" s="7"/>
+      <c r="B96" s="6"/>
     </row>
     <row r="97" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B97" s="7"/>
+      <c r="B97" s="6"/>
     </row>
     <row r="98" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B98" s="7"/>
+      <c r="B98" s="6"/>
     </row>
     <row r="99" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B99" s="7"/>
+      <c r="B99" s="6"/>
     </row>
     <row r="100" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B100" s="7"/>
+      <c r="B100" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5602,247 +5572,247 @@
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
     </row>
     <row r="22" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B30" s="7"/>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B34" s="7"/>
+      <c r="B34" s="6"/>
     </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B35" s="7"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B36" s="7"/>
+      <c r="B36" s="6"/>
     </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B37" s="7"/>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B39" s="7"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B40" s="7"/>
+      <c r="B40" s="6"/>
     </row>
     <row r="41" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B41" s="7"/>
+      <c r="B41" s="6"/>
     </row>
     <row r="42" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B42" s="7"/>
+      <c r="B42" s="6"/>
     </row>
     <row r="43" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B43" s="7"/>
+      <c r="B43" s="6"/>
     </row>
     <row r="44" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B44" s="7"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B45" s="7"/>
+      <c r="B45" s="6"/>
     </row>
     <row r="46" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B46" s="7"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B48" s="7"/>
+      <c r="B48" s="6"/>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B49" s="7"/>
+      <c r="B49" s="6"/>
     </row>
     <row r="50" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B50" s="7"/>
+      <c r="B50" s="6"/>
     </row>
     <row r="51" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
     </row>
     <row r="52" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B52" s="7"/>
+      <c r="B52" s="6"/>
     </row>
     <row r="53" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B53" s="7"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B54" s="7"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B55" s="7"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B56" s="7"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B57" s="7"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B58" s="7"/>
+      <c r="B58" s="6"/>
     </row>
     <row r="59" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B59" s="7"/>
+      <c r="B59" s="6"/>
     </row>
     <row r="60" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B60" s="7"/>
+      <c r="B60" s="6"/>
     </row>
     <row r="61" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B61" s="7"/>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B62" s="7"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B63" s="7"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B64" s="7"/>
+      <c r="B64" s="6"/>
     </row>
     <row r="65" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B65" s="7"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B66" s="7"/>
+      <c r="B66" s="6"/>
     </row>
     <row r="67" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B67" s="7"/>
+      <c r="B67" s="6"/>
     </row>
     <row r="68" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B68" s="7"/>
+      <c r="B68" s="6"/>
     </row>
     <row r="69" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B69" s="7"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B70" s="7"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B71" s="7"/>
+      <c r="B71" s="6"/>
     </row>
     <row r="72" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B72" s="7"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B73" s="7"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B74" s="7"/>
+      <c r="B74" s="6"/>
     </row>
     <row r="75" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B75" s="7"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B76" s="7"/>
+      <c r="B76" s="6"/>
     </row>
     <row r="77" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B77" s="7"/>
+      <c r="B77" s="6"/>
     </row>
     <row r="78" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B78" s="7"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B79" s="7"/>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B80" s="7"/>
+      <c r="B80" s="6"/>
     </row>
     <row r="81" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B81" s="7"/>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B82" s="7"/>
+      <c r="B82" s="6"/>
     </row>
     <row r="83" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B83" s="7"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B84" s="7"/>
+      <c r="B84" s="6"/>
     </row>
     <row r="85" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B85" s="7"/>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B86" s="7"/>
+      <c r="B86" s="6"/>
     </row>
     <row r="87" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B87" s="7"/>
+      <c r="B87" s="6"/>
     </row>
     <row r="88" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B88" s="7"/>
+      <c r="B88" s="6"/>
     </row>
     <row r="89" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B89" s="7"/>
+      <c r="B89" s="6"/>
     </row>
     <row r="90" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B90" s="7"/>
+      <c r="B90" s="6"/>
     </row>
     <row r="91" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B91" s="7"/>
+      <c r="B91" s="6"/>
     </row>
     <row r="92" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B92" s="7"/>
+      <c r="B92" s="6"/>
     </row>
     <row r="93" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B93" s="7"/>
+      <c r="B93" s="6"/>
     </row>
     <row r="94" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B94" s="7"/>
+      <c r="B94" s="6"/>
     </row>
     <row r="95" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B95" s="7"/>
+      <c r="B95" s="6"/>
     </row>
     <row r="96" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B96" s="7"/>
+      <c r="B96" s="6"/>
     </row>
     <row r="97" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B97" s="7"/>
+      <c r="B97" s="6"/>
     </row>
     <row r="98" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B98" s="7"/>
+      <c r="B98" s="6"/>
     </row>
     <row r="99" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B99" s="7"/>
+      <c r="B99" s="6"/>
     </row>
     <row r="100" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B100" s="7"/>
+      <c r="B100" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>